<commit_message>
Added the cache impact graph and wrote the text for future prediction experiment
</commit_message>
<xml_diff>
--- a/paper/raw_data/results_HBM2_DDR41600_and_offline.xlsx
+++ b/paper/raw_data/results_HBM2_DDR41600_and_offline.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prodr\Desktop\NLM\MemPod\paper_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prodr\Desktop\NLM\MemPod\paper\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20085" windowHeight="2970" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20085" windowHeight="2970" firstSheet="8" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="exp17" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,10 @@
     <sheet name="exp29_counting" sheetId="13" r:id="rId13"/>
     <sheet name="exp29_future" sheetId="14" r:id="rId14"/>
     <sheet name="exp26" sheetId="17" r:id="rId15"/>
+    <sheet name="exp30" sheetId="20" r:id="rId16"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="91">
   <si>
     <t>BENCH</t>
   </si>
@@ -285,6 +286,36 @@
   <si>
     <t>NO CACHE</t>
   </si>
+  <si>
+    <t>AVG AMMT</t>
+  </si>
+  <si>
+    <t>HMA-0.05</t>
+  </si>
+  <si>
+    <t>HMA-0.01</t>
+  </si>
+  <si>
+    <t>HMA-ORACLE</t>
+  </si>
+  <si>
+    <t>64kB</t>
+  </si>
+  <si>
+    <t>32kB</t>
+  </si>
+  <si>
+    <t>16kB</t>
+  </si>
+  <si>
+    <t>HMA 0.05</t>
+  </si>
+  <si>
+    <t>HMA 0.01</t>
+  </si>
+  <si>
+    <t>HMA OCL</t>
+  </si>
 </sst>
 </file>
 
@@ -387,6 +418,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -405,7 +437,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,7 +491,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1782,11 +1812,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-258527152"/>
-        <c:axId val="-258534224"/>
+        <c:axId val="-2010985744"/>
+        <c:axId val="-2010984656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-258527152"/>
+        <c:axId val="-2010985744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1826,7 +1856,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-258534224"/>
+        <c:crossAx val="-2010984656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1834,7 +1864,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-258534224"/>
+        <c:axId val="-2010984656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1877,7 +1907,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1932,7 +1961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-258527152"/>
+        <c:crossAx val="-2010985744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1946,7 +1975,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2051,7 +2079,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3416,8 +3443,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-146327040"/>
-        <c:axId val="-146326496"/>
+        <c:axId val="-144864448"/>
+        <c:axId val="-144871520"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4372,11 +4399,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-542789008"/>
-        <c:axId val="-146333568"/>
+        <c:axId val="-144860640"/>
+        <c:axId val="-144868256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-146327040"/>
+        <c:axId val="-144864448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4405,7 +4432,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4465,7 +4491,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-146326496"/>
+        <c:crossAx val="-144871520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4473,7 +4499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-146326496"/>
+        <c:axId val="-144871520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4516,7 +4542,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4571,12 +4596,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-146327040"/>
+        <c:crossAx val="-144864448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-146333568"/>
+        <c:axId val="-144868256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4605,7 +4630,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4660,12 +4684,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-542789008"/>
+        <c:crossAx val="-144860640"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-542789008"/>
+        <c:axId val="-144860640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4704,7 +4728,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-146333568"/>
+        <c:crossAx val="-144868256"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4841,7 +4865,6 @@
         <c:idx val="31"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6486,8 +6509,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-542790096"/>
-        <c:axId val="-542787920"/>
+        <c:axId val="-144856832"/>
+        <c:axId val="-144856288"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7589,11 +7612,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-386600064"/>
-        <c:axId val="-542787376"/>
+        <c:axId val="-57110928"/>
+        <c:axId val="-144855200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-542790096"/>
+        <c:axId val="-144856832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7681,7 +7704,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-542787920"/>
+        <c:crossAx val="-144856288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7689,7 +7712,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-542787920"/>
+        <c:axId val="-144856288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.05"/>
@@ -7793,12 +7816,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-542790096"/>
+        <c:crossAx val="-144856832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-542787376"/>
+        <c:axId val="-144855200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7881,12 +7904,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-386600064"/>
+        <c:crossAx val="-57110928"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-386600064"/>
+        <c:axId val="-57110928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7925,7 +7948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-542787376"/>
+        <c:crossAx val="-144855200"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9461,8 +9484,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-386603872"/>
-        <c:axId val="-386603328"/>
+        <c:axId val="-57119632"/>
+        <c:axId val="-57119088"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -10372,11 +10395,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-386604416"/>
-        <c:axId val="-386601696"/>
+        <c:axId val="-57112560"/>
+        <c:axId val="-57116912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-386603872"/>
+        <c:axId val="-57119632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10474,7 +10497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-386603328"/>
+        <c:crossAx val="-57119088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10482,7 +10505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-386603328"/>
+        <c:axId val="-57119088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10589,12 +10612,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-386603872"/>
+        <c:crossAx val="-57119632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-386601696"/>
+        <c:axId val="-57116912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10687,12 +10710,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-386604416"/>
+        <c:crossAx val="-57112560"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-386604416"/>
+        <c:axId val="-57112560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10734,7 +10757,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-386601696"/>
+        <c:crossAx val="-57116912"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12386,8 +12409,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-386600608"/>
-        <c:axId val="-386604960"/>
+        <c:axId val="-57120720"/>
+        <c:axId val="-57118544"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -13441,11 +13464,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-386598432"/>
-        <c:axId val="-386598976"/>
+        <c:axId val="-57113648"/>
+        <c:axId val="-57120176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-386600608"/>
+        <c:axId val="-57120720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13534,7 +13557,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-386604960"/>
+        <c:crossAx val="-57118544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13542,7 +13565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-386604960"/>
+        <c:axId val="-57118544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13640,13 +13663,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-386600608"/>
+        <c:crossAx val="-57120720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-386598976"/>
+        <c:axId val="-57120176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10"/>
@@ -13731,12 +13754,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-386598432"/>
+        <c:crossAx val="-57113648"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-386598432"/>
+        <c:axId val="-57113648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13775,7 +13798,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-386598976"/>
+        <c:crossAx val="-57120176"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14706,11 +14729,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-370553856"/>
-        <c:axId val="-370555488"/>
+        <c:axId val="-2010107536"/>
+        <c:axId val="-2010104272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-370553856"/>
+        <c:axId val="-2010107536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14753,7 +14776,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-370555488"/>
+        <c:crossAx val="-2010104272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14761,7 +14784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-370555488"/>
+        <c:axId val="-2010104272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14812,7 +14835,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-370553856"/>
+        <c:crossAx val="-2010107536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15741,11 +15764,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-370560928"/>
-        <c:axId val="-380410960"/>
+        <c:axId val="-2010103728"/>
+        <c:axId val="-2010102096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-370560928"/>
+        <c:axId val="-2010103728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15785,7 +15808,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-380410960"/>
+        <c:crossAx val="-2010102096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15793,7 +15816,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-380410960"/>
+        <c:axId val="-2010102096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15841,7 +15864,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-370560928"/>
+        <c:crossAx val="-2010103728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16807,11 +16830,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-380407696"/>
-        <c:axId val="-380409328"/>
+        <c:axId val="-2010101008"/>
+        <c:axId val="-2010100464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-380407696"/>
+        <c:axId val="-2010101008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16851,7 +16874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-380409328"/>
+        <c:crossAx val="-2010100464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16859,7 +16882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-380409328"/>
+        <c:axId val="-2010100464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16907,7 +16930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-380407696"/>
+        <c:crossAx val="-2010101008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17736,11 +17759,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-380408784"/>
-        <c:axId val="-380410416"/>
+        <c:axId val="-155677184"/>
+        <c:axId val="-155667936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-380408784"/>
+        <c:axId val="-155677184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17780,7 +17803,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-380410416"/>
+        <c:crossAx val="-155667936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17788,7 +17811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-380410416"/>
+        <c:axId val="-155667936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17886,7 +17909,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-380408784"/>
+        <c:crossAx val="-155677184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17964,6 +17987,393 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'exp30'!$A$73</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG AMMT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'exp30'!$B$71:$P$72</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>HMA OCL</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>MP</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>HMA 0.01</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>THM</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>HMA 0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>HMA OCL</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>MP</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>HMA 0.01</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>THM</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>HMA 0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>HMA OCL</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>MP</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>HMA 0.01</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>THM</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>HMA 0.05</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>16kB</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>32kB</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>64kB</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'exp30'!$B$73:$P$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>29.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.86</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.76</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.91</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.97</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.229999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>49.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35.119999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>51.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="55"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-144199920"/>
+        <c:axId val="-144201008"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-144199920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-144201008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-144201008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>AVG AMMT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-144199920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -18687,11 +19097,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-258528240"/>
-        <c:axId val="-258532592"/>
+        <c:axId val="-2010992816"/>
+        <c:axId val="-2010984112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-258528240"/>
+        <c:axId val="-2010992816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18731,7 +19141,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-258532592"/>
+        <c:crossAx val="-2010984112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18739,7 +19149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-258532592"/>
+        <c:axId val="-2010984112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18787,7 +19197,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-258528240"/>
+        <c:crossAx val="-2010992816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19837,11 +20247,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-258533136"/>
-        <c:axId val="-258531504"/>
+        <c:axId val="-2010983024"/>
+        <c:axId val="-2010982480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-258533136"/>
+        <c:axId val="-2010983024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19881,7 +20291,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-258531504"/>
+        <c:crossAx val="-2010982480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19889,7 +20299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-258531504"/>
+        <c:axId val="-2010982480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19987,7 +20397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-258533136"/>
+        <c:crossAx val="-2010983024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20106,7 +20516,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -20942,11 +21351,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-377244192"/>
-        <c:axId val="-377243648"/>
+        <c:axId val="-2010994992"/>
+        <c:axId val="-2010994448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-377244192"/>
+        <c:axId val="-2010994992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20986,7 +21395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-377243648"/>
+        <c:crossAx val="-2010994448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20994,7 +21403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-377243648"/>
+        <c:axId val="-2010994448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21042,7 +21451,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-377244192"/>
+        <c:crossAx val="-2010994992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21056,7 +21465,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21161,7 +21569,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21997,11 +22404,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-377247456"/>
-        <c:axId val="-377248544"/>
+        <c:axId val="-2010992272"/>
+        <c:axId val="-2010991728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-377247456"/>
+        <c:axId val="-2010992272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22041,7 +22448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-377248544"/>
+        <c:crossAx val="-2010991728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22049,7 +22456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-377248544"/>
+        <c:axId val="-2010991728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22097,7 +22504,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-377247456"/>
+        <c:crossAx val="-2010992272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22111,7 +22518,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22216,7 +22622,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23579,8 +23984,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-377249632"/>
-        <c:axId val="-377246368"/>
+        <c:axId val="-2010990640"/>
+        <c:axId val="-2010990096"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -24533,11 +24938,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-276837664"/>
-        <c:axId val="-377245280"/>
+        <c:axId val="-144880768"/>
+        <c:axId val="-2010988464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-377249632"/>
+        <c:axId val="-2010990640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24566,7 +24971,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -24626,7 +25030,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-377246368"/>
+        <c:crossAx val="-2010990096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24634,7 +25038,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-377246368"/>
+        <c:axId val="-2010990096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24677,7 +25081,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -24732,12 +25135,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-377249632"/>
+        <c:crossAx val="-2010990640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-377245280"/>
+        <c:axId val="-2010988464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24771,7 +25174,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -24826,12 +25228,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-276837664"/>
+        <c:crossAx val="-144880768"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-276837664"/>
+        <c:axId val="-144880768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24870,7 +25272,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-377245280"/>
+        <c:crossAx val="-2010988464"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25007,7 +25409,6 @@
         <c:idx val="31"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25125,7 +25526,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26626,8 +27026,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-276834944"/>
-        <c:axId val="-276836576"/>
+        <c:axId val="-144858464"/>
+        <c:axId val="-144879136"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -27726,11 +28126,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-276833856"/>
-        <c:axId val="-276832768"/>
+        <c:axId val="-144870976"/>
+        <c:axId val="-144862816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-276834944"/>
+        <c:axId val="-144858464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27831,7 +28231,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-276836576"/>
+        <c:crossAx val="-144879136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -27839,7 +28239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-276836576"/>
+        <c:axId val="-144879136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.85000000000000009"/>
@@ -27883,7 +28283,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -27938,13 +28337,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-276834944"/>
+        <c:crossAx val="-144858464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-276832768"/>
+        <c:axId val="-144862816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27973,7 +28372,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -28028,12 +28426,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-276833856"/>
+        <c:crossAx val="-144870976"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-276833856"/>
+        <c:axId val="-144870976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28072,7 +28470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-276832768"/>
+        <c:crossAx val="-144862816"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28323,7 +28721,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -29699,11 +30096,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-276836032"/>
-        <c:axId val="-276831680"/>
+        <c:axId val="-144884032"/>
+        <c:axId val="-144872608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-276836032"/>
+        <c:axId val="-144884032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29743,7 +30140,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-276831680"/>
+        <c:crossAx val="-144872608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -29751,7 +30148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-276831680"/>
+        <c:axId val="-144872608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29794,7 +30191,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -29849,7 +30245,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-276836032"/>
+        <c:crossAx val="-144884032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -29863,7 +30259,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -31343,11 +31738,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-146329760"/>
-        <c:axId val="-146328128"/>
+        <c:axId val="-144872064"/>
+        <c:axId val="-144864992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-146329760"/>
+        <c:axId val="-144872064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -31387,7 +31782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-146328128"/>
+        <c:crossAx val="-144864992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -31395,7 +31790,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-146328128"/>
+        <c:axId val="-144864992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -31492,7 +31887,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-146329760"/>
+        <c:crossAx val="-144872064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -31894,6 +32289,46 @@
 </file>
 
 <file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -36832,6 +37267,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -41118,6 +42056,43 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -42216,22 +43191,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -42250,22 +43225,22 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -43503,35 +44478,35 @@
       <c r="A33" s="4"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
@@ -46152,13 +47127,13 @@
       <c r="L2" s="4">
         <v>32</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
@@ -48504,69 +49479,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="14" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14" t="s">
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="12" t="s">
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
       <c r="V4" s="4"/>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4" t="s">
@@ -50760,40 +51735,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -53409,17 +54384,17 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -55318,12 +56293,2120 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="M72" sqref="M72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>35.82</v>
+      </c>
+      <c r="C3">
+        <v>35.72</v>
+      </c>
+      <c r="D3">
+        <v>35.619999999999997</v>
+      </c>
+      <c r="E3">
+        <v>35.65</v>
+      </c>
+      <c r="F3">
+        <v>35.53</v>
+      </c>
+      <c r="G3">
+        <v>35.32</v>
+      </c>
+      <c r="H3">
+        <v>25.46</v>
+      </c>
+      <c r="I3">
+        <v>25.43</v>
+      </c>
+      <c r="J3">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>49.97</v>
+      </c>
+      <c r="C4">
+        <v>49.86</v>
+      </c>
+      <c r="D4">
+        <v>49.83</v>
+      </c>
+      <c r="E4">
+        <v>53.66</v>
+      </c>
+      <c r="F4">
+        <v>53.65</v>
+      </c>
+      <c r="G4">
+        <v>53.63</v>
+      </c>
+      <c r="H4">
+        <v>44.73</v>
+      </c>
+      <c r="I4">
+        <v>44.73</v>
+      </c>
+      <c r="J4">
+        <v>44.73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>79.22</v>
+      </c>
+      <c r="C5">
+        <v>77.91</v>
+      </c>
+      <c r="D5">
+        <v>75.959999999999994</v>
+      </c>
+      <c r="E5">
+        <v>81.12</v>
+      </c>
+      <c r="F5">
+        <v>79.760000000000005</v>
+      </c>
+      <c r="G5">
+        <v>77.739999999999995</v>
+      </c>
+      <c r="H5">
+        <v>67.459999999999994</v>
+      </c>
+      <c r="I5">
+        <v>67.06</v>
+      </c>
+      <c r="J5">
+        <v>66.87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>52.15</v>
+      </c>
+      <c r="C6">
+        <v>45.91</v>
+      </c>
+      <c r="D6">
+        <v>45.59</v>
+      </c>
+      <c r="E6">
+        <v>55.39</v>
+      </c>
+      <c r="F6">
+        <v>47.83</v>
+      </c>
+      <c r="G6">
+        <v>47.71</v>
+      </c>
+      <c r="H6">
+        <v>50.02</v>
+      </c>
+      <c r="I6">
+        <v>49.73</v>
+      </c>
+      <c r="J6">
+        <v>49.74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>74.67</v>
+      </c>
+      <c r="C7">
+        <v>73.72</v>
+      </c>
+      <c r="D7">
+        <v>72.930000000000007</v>
+      </c>
+      <c r="E7">
+        <v>80.790000000000006</v>
+      </c>
+      <c r="F7">
+        <v>79.84</v>
+      </c>
+      <c r="G7">
+        <v>78.95</v>
+      </c>
+      <c r="H7">
+        <v>70.89</v>
+      </c>
+      <c r="I7">
+        <v>70.75</v>
+      </c>
+      <c r="J7">
+        <v>70.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8">
+        <v>21.02</v>
+      </c>
+      <c r="C8">
+        <v>20.85</v>
+      </c>
+      <c r="D8">
+        <v>20.71</v>
+      </c>
+      <c r="F8">
+        <v>24.53</v>
+      </c>
+      <c r="G8">
+        <v>24.35</v>
+      </c>
+      <c r="H8">
+        <v>17.75</v>
+      </c>
+      <c r="I8">
+        <v>17.7</v>
+      </c>
+      <c r="J8">
+        <v>17.61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>53.82</v>
+      </c>
+      <c r="E9">
+        <v>51.91</v>
+      </c>
+      <c r="F9">
+        <v>51.48</v>
+      </c>
+      <c r="H9">
+        <v>52.12</v>
+      </c>
+      <c r="J9">
+        <v>52.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>20.03</v>
+      </c>
+      <c r="C10">
+        <v>19.88</v>
+      </c>
+      <c r="D10">
+        <v>19.47</v>
+      </c>
+      <c r="E10">
+        <v>23.26</v>
+      </c>
+      <c r="F10">
+        <v>23.12</v>
+      </c>
+      <c r="G10">
+        <v>22.57</v>
+      </c>
+      <c r="H10">
+        <v>25.79</v>
+      </c>
+      <c r="I10">
+        <v>25.8</v>
+      </c>
+      <c r="J10">
+        <v>25.81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>39.61</v>
+      </c>
+      <c r="C11">
+        <v>38.869999999999997</v>
+      </c>
+      <c r="D11">
+        <v>38.71</v>
+      </c>
+      <c r="E11">
+        <v>43.38</v>
+      </c>
+      <c r="F11">
+        <v>42.64</v>
+      </c>
+      <c r="G11">
+        <v>42.46</v>
+      </c>
+      <c r="H11">
+        <v>43.74</v>
+      </c>
+      <c r="I11">
+        <v>43.61</v>
+      </c>
+      <c r="J11">
+        <v>43.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>15.89</v>
+      </c>
+      <c r="C12">
+        <v>15.87</v>
+      </c>
+      <c r="D12">
+        <v>15.87</v>
+      </c>
+      <c r="E12">
+        <v>20.079999999999998</v>
+      </c>
+      <c r="F12">
+        <v>20.07</v>
+      </c>
+      <c r="G12">
+        <v>20.04</v>
+      </c>
+      <c r="H12">
+        <v>14.92</v>
+      </c>
+      <c r="I12">
+        <v>14.88</v>
+      </c>
+      <c r="J12">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13">
+        <v>31.27</v>
+      </c>
+      <c r="F13">
+        <v>31.23</v>
+      </c>
+      <c r="G13">
+        <v>31.15</v>
+      </c>
+      <c r="H13">
+        <v>25.31</v>
+      </c>
+      <c r="I13">
+        <v>25.31</v>
+      </c>
+      <c r="J13">
+        <v>25.31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>36.64</v>
+      </c>
+      <c r="C14">
+        <v>36.39</v>
+      </c>
+      <c r="D14">
+        <v>36.06</v>
+      </c>
+      <c r="E14">
+        <v>41.5</v>
+      </c>
+      <c r="F14">
+        <v>41.24</v>
+      </c>
+      <c r="H14">
+        <v>33.93</v>
+      </c>
+      <c r="J14">
+        <v>33.909999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>24.76</v>
+      </c>
+      <c r="C15">
+        <v>24.51</v>
+      </c>
+      <c r="D15">
+        <v>24.02</v>
+      </c>
+      <c r="E15">
+        <v>28.42</v>
+      </c>
+      <c r="F15">
+        <v>28.16</v>
+      </c>
+      <c r="H15">
+        <v>21.94</v>
+      </c>
+      <c r="I15">
+        <v>21.92</v>
+      </c>
+      <c r="J15">
+        <v>21.87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>45.09</v>
+      </c>
+      <c r="D16">
+        <v>44.51</v>
+      </c>
+      <c r="E16">
+        <v>47.07</v>
+      </c>
+      <c r="F16">
+        <v>46.78</v>
+      </c>
+      <c r="G16">
+        <v>46.44</v>
+      </c>
+      <c r="I16">
+        <v>39.11</v>
+      </c>
+      <c r="J16">
+        <v>39.049999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>55.42</v>
+      </c>
+      <c r="C17">
+        <v>54.13</v>
+      </c>
+      <c r="D17">
+        <v>53.26</v>
+      </c>
+      <c r="E17">
+        <v>59.82</v>
+      </c>
+      <c r="F17">
+        <v>58.69</v>
+      </c>
+      <c r="G17">
+        <v>57.79</v>
+      </c>
+      <c r="H17">
+        <v>53.6</v>
+      </c>
+      <c r="I17">
+        <v>53.46</v>
+      </c>
+      <c r="J17">
+        <v>53.38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>44.33</v>
+      </c>
+      <c r="C18">
+        <v>43.94</v>
+      </c>
+      <c r="D18">
+        <v>43.54</v>
+      </c>
+      <c r="E18">
+        <v>46.62</v>
+      </c>
+      <c r="I18">
+        <v>37.6</v>
+      </c>
+      <c r="J18">
+        <v>37.56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>27.88</v>
+      </c>
+      <c r="C19">
+        <v>27.58</v>
+      </c>
+      <c r="D19">
+        <v>27</v>
+      </c>
+      <c r="E19">
+        <v>32.47</v>
+      </c>
+      <c r="F19">
+        <v>32.17</v>
+      </c>
+      <c r="G19">
+        <v>31.46</v>
+      </c>
+      <c r="H19">
+        <v>25.77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>41.24</v>
+      </c>
+      <c r="D20">
+        <v>40.409999999999997</v>
+      </c>
+      <c r="E20">
+        <v>47.37</v>
+      </c>
+      <c r="F20">
+        <v>46.5</v>
+      </c>
+      <c r="G20">
+        <v>45.72</v>
+      </c>
+      <c r="H20">
+        <v>33.93</v>
+      </c>
+      <c r="I20">
+        <v>33.840000000000003</v>
+      </c>
+      <c r="J20">
+        <v>33.770000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>43.75</v>
+      </c>
+      <c r="C21">
+        <v>41.69</v>
+      </c>
+      <c r="D21">
+        <v>40.22</v>
+      </c>
+      <c r="E21">
+        <v>48.1</v>
+      </c>
+      <c r="F21">
+        <v>46.08</v>
+      </c>
+      <c r="G21">
+        <v>44.55</v>
+      </c>
+      <c r="H21">
+        <v>37.950000000000003</v>
+      </c>
+      <c r="I21">
+        <v>37.770000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>33.78</v>
+      </c>
+      <c r="C22">
+        <v>32.67</v>
+      </c>
+      <c r="E22">
+        <v>36.9</v>
+      </c>
+      <c r="F22">
+        <v>35.840000000000003</v>
+      </c>
+      <c r="G22">
+        <v>34.729999999999997</v>
+      </c>
+      <c r="I22">
+        <v>31.43</v>
+      </c>
+      <c r="J22">
+        <v>31.34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>52.82</v>
+      </c>
+      <c r="C23">
+        <v>52.26</v>
+      </c>
+      <c r="D23">
+        <v>51.37</v>
+      </c>
+      <c r="G23">
+        <v>53.65</v>
+      </c>
+      <c r="H23">
+        <v>47.95</v>
+      </c>
+      <c r="J23">
+        <v>47.85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>46.98</v>
+      </c>
+      <c r="D24">
+        <v>45.66</v>
+      </c>
+      <c r="F24">
+        <v>53.28</v>
+      </c>
+      <c r="G24">
+        <v>52.74</v>
+      </c>
+      <c r="H24">
+        <v>41.74</v>
+      </c>
+      <c r="J24">
+        <v>41.61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <v>45.65</v>
+      </c>
+      <c r="D25">
+        <v>45.33</v>
+      </c>
+      <c r="E25">
+        <v>48.98</v>
+      </c>
+      <c r="G25">
+        <v>48.17</v>
+      </c>
+      <c r="H25">
+        <v>40.46</v>
+      </c>
+      <c r="I25">
+        <v>40.43</v>
+      </c>
+      <c r="J25">
+        <v>40.369999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>36.97</v>
+      </c>
+      <c r="C26">
+        <v>36.68</v>
+      </c>
+      <c r="D26">
+        <v>36.51</v>
+      </c>
+      <c r="E26">
+        <v>42.91</v>
+      </c>
+      <c r="F26">
+        <v>42.61</v>
+      </c>
+      <c r="G26">
+        <v>42.32</v>
+      </c>
+      <c r="H26">
+        <v>25.59</v>
+      </c>
+      <c r="I26">
+        <v>25.54</v>
+      </c>
+      <c r="J26">
+        <v>25.49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>21.18</v>
+      </c>
+      <c r="C27">
+        <v>20.56</v>
+      </c>
+      <c r="D27">
+        <v>19.79</v>
+      </c>
+      <c r="E27">
+        <v>23.63</v>
+      </c>
+      <c r="F27">
+        <v>23.01</v>
+      </c>
+      <c r="G27">
+        <v>22.2</v>
+      </c>
+      <c r="H27">
+        <v>15.51</v>
+      </c>
+      <c r="I27">
+        <v>15.31</v>
+      </c>
+      <c r="J27">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="C28">
+        <v>34.24</v>
+      </c>
+      <c r="D28">
+        <v>33.85</v>
+      </c>
+      <c r="E28">
+        <v>37</v>
+      </c>
+      <c r="G28">
+        <v>36.14</v>
+      </c>
+      <c r="H28">
+        <v>32.1</v>
+      </c>
+      <c r="I28">
+        <v>32</v>
+      </c>
+      <c r="J28">
+        <v>31.88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29">
+        <v>76.98</v>
+      </c>
+      <c r="E29">
+        <v>85.34</v>
+      </c>
+      <c r="F29">
+        <v>84.65</v>
+      </c>
+      <c r="G29">
+        <v>84.06</v>
+      </c>
+      <c r="H29">
+        <v>71.28</v>
+      </c>
+      <c r="I29">
+        <v>71.14</v>
+      </c>
+      <c r="J29">
+        <v>71.040000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>57.3</v>
+      </c>
+      <c r="C30">
+        <v>57.11</v>
+      </c>
+      <c r="D30">
+        <v>56.77</v>
+      </c>
+      <c r="E30">
+        <v>60.68</v>
+      </c>
+      <c r="F30">
+        <v>60.43</v>
+      </c>
+      <c r="G30">
+        <v>60</v>
+      </c>
+      <c r="H30">
+        <v>59.11</v>
+      </c>
+      <c r="I30">
+        <v>59.12</v>
+      </c>
+      <c r="J30">
+        <v>59.23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="F37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="K37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L37" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>35.82</v>
+      </c>
+      <c r="C39">
+        <v>35.72</v>
+      </c>
+      <c r="D39">
+        <v>35.619999999999997</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39">
+        <v>35.65</v>
+      </c>
+      <c r="H39">
+        <v>35.53</v>
+      </c>
+      <c r="I39">
+        <v>35.32</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L39">
+        <v>25.46</v>
+      </c>
+      <c r="M39">
+        <v>25.43</v>
+      </c>
+      <c r="N39">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40">
+        <v>49.97</v>
+      </c>
+      <c r="C40">
+        <v>49.86</v>
+      </c>
+      <c r="D40">
+        <v>49.83</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40">
+        <v>53.66</v>
+      </c>
+      <c r="H40">
+        <v>53.65</v>
+      </c>
+      <c r="I40">
+        <v>53.63</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40">
+        <v>44.73</v>
+      </c>
+      <c r="M40">
+        <v>44.73</v>
+      </c>
+      <c r="N40">
+        <v>44.73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41">
+        <v>79.22</v>
+      </c>
+      <c r="C41">
+        <v>77.91</v>
+      </c>
+      <c r="D41">
+        <v>75.959999999999994</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41">
+        <v>81.12</v>
+      </c>
+      <c r="H41">
+        <v>79.760000000000005</v>
+      </c>
+      <c r="I41">
+        <v>77.739999999999995</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L41">
+        <v>67.459999999999994</v>
+      </c>
+      <c r="M41">
+        <v>67.06</v>
+      </c>
+      <c r="N41">
+        <v>66.87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>52.15</v>
+      </c>
+      <c r="C42">
+        <v>45.91</v>
+      </c>
+      <c r="D42">
+        <v>45.59</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42">
+        <v>55.39</v>
+      </c>
+      <c r="H42">
+        <v>47.83</v>
+      </c>
+      <c r="I42">
+        <v>47.71</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L42">
+        <v>50.02</v>
+      </c>
+      <c r="M42">
+        <v>49.73</v>
+      </c>
+      <c r="N42">
+        <v>49.74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>74.67</v>
+      </c>
+      <c r="C43">
+        <v>73.72</v>
+      </c>
+      <c r="D43">
+        <v>72.930000000000007</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43">
+        <v>80.790000000000006</v>
+      </c>
+      <c r="H43">
+        <v>79.84</v>
+      </c>
+      <c r="I43">
+        <v>78.95</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43">
+        <v>70.89</v>
+      </c>
+      <c r="M43">
+        <v>70.75</v>
+      </c>
+      <c r="N43">
+        <v>70.59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>21.02</v>
+      </c>
+      <c r="C44">
+        <v>20.85</v>
+      </c>
+      <c r="D44">
+        <v>20.71</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44">
+        <v>23.26</v>
+      </c>
+      <c r="H44">
+        <v>23.12</v>
+      </c>
+      <c r="I44">
+        <v>22.57</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L44">
+        <v>17.75</v>
+      </c>
+      <c r="M44">
+        <v>17.7</v>
+      </c>
+      <c r="N44">
+        <v>17.61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>20.03</v>
+      </c>
+      <c r="C45">
+        <v>19.88</v>
+      </c>
+      <c r="D45">
+        <v>19.47</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45">
+        <v>43.38</v>
+      </c>
+      <c r="H45">
+        <v>42.64</v>
+      </c>
+      <c r="I45">
+        <v>42.46</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L45">
+        <v>25.79</v>
+      </c>
+      <c r="M45">
+        <v>25.8</v>
+      </c>
+      <c r="N45">
+        <v>25.81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>39.61</v>
+      </c>
+      <c r="C46">
+        <v>38.869999999999997</v>
+      </c>
+      <c r="D46">
+        <v>38.71</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46">
+        <v>20.079999999999998</v>
+      </c>
+      <c r="H46">
+        <v>20.07</v>
+      </c>
+      <c r="I46">
+        <v>20.04</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L46">
+        <v>43.74</v>
+      </c>
+      <c r="M46">
+        <v>43.61</v>
+      </c>
+      <c r="N46">
+        <v>43.48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47">
+        <v>15.89</v>
+      </c>
+      <c r="C47">
+        <v>15.87</v>
+      </c>
+      <c r="D47">
+        <v>15.87</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G47">
+        <v>31.27</v>
+      </c>
+      <c r="H47">
+        <v>31.23</v>
+      </c>
+      <c r="I47">
+        <v>31.15</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L47">
+        <v>14.92</v>
+      </c>
+      <c r="M47">
+        <v>14.88</v>
+      </c>
+      <c r="N47">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48">
+        <v>36.97</v>
+      </c>
+      <c r="C48">
+        <v>36.68</v>
+      </c>
+      <c r="D48">
+        <v>36.51</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48">
+        <v>42.91</v>
+      </c>
+      <c r="H48">
+        <v>42.61</v>
+      </c>
+      <c r="I48">
+        <v>42.32</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L48">
+        <v>25.31</v>
+      </c>
+      <c r="M48">
+        <v>25.31</v>
+      </c>
+      <c r="N48">
+        <v>25.31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49">
+        <v>21.18</v>
+      </c>
+      <c r="C49">
+        <v>20.56</v>
+      </c>
+      <c r="D49">
+        <v>19.79</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49">
+        <v>23.63</v>
+      </c>
+      <c r="H49">
+        <v>23.01</v>
+      </c>
+      <c r="I49">
+        <v>22.2</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L49">
+        <v>25.59</v>
+      </c>
+      <c r="M49">
+        <v>25.54</v>
+      </c>
+      <c r="N49">
+        <v>25.49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="C50">
+        <v>34.24</v>
+      </c>
+      <c r="D50">
+        <v>33.85</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G50">
+        <v>85.34</v>
+      </c>
+      <c r="H50">
+        <v>84.65</v>
+      </c>
+      <c r="I50">
+        <v>84.06</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L50">
+        <v>15.51</v>
+      </c>
+      <c r="M50">
+        <v>15.31</v>
+      </c>
+      <c r="N50">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51">
+        <v>57.3</v>
+      </c>
+      <c r="C51">
+        <v>57.11</v>
+      </c>
+      <c r="D51">
+        <v>56.77</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51">
+        <v>60.68</v>
+      </c>
+      <c r="H51">
+        <v>60.43</v>
+      </c>
+      <c r="I51">
+        <v>60</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L51">
+        <v>32.1</v>
+      </c>
+      <c r="M51">
+        <v>32</v>
+      </c>
+      <c r="N51">
+        <v>31.88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52">
+        <v>36.64</v>
+      </c>
+      <c r="C52">
+        <v>36.39</v>
+      </c>
+      <c r="D52">
+        <v>36.06</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52">
+        <v>32.47</v>
+      </c>
+      <c r="H52">
+        <v>32.17</v>
+      </c>
+      <c r="I52">
+        <v>31.46</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L52">
+        <v>71.28</v>
+      </c>
+      <c r="M52">
+        <v>71.14</v>
+      </c>
+      <c r="N52">
+        <v>71.040000000000006</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53">
+        <v>44.33</v>
+      </c>
+      <c r="C53">
+        <v>43.94</v>
+      </c>
+      <c r="D53">
+        <v>43.54</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53">
+        <v>47.37</v>
+      </c>
+      <c r="H53">
+        <v>46.5</v>
+      </c>
+      <c r="I53">
+        <v>45.72</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L53">
+        <v>59.11</v>
+      </c>
+      <c r="M53">
+        <v>59.12</v>
+      </c>
+      <c r="N53">
+        <v>59.23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54">
+        <v>27.88</v>
+      </c>
+      <c r="C54">
+        <v>27.58</v>
+      </c>
+      <c r="D54">
+        <v>27</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G54">
+        <v>48.1</v>
+      </c>
+      <c r="H54">
+        <v>46.08</v>
+      </c>
+      <c r="I54">
+        <v>44.55</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L54">
+        <v>33.93</v>
+      </c>
+      <c r="M54">
+        <v>33.840000000000003</v>
+      </c>
+      <c r="N54">
+        <v>33.770000000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55">
+        <v>43.75</v>
+      </c>
+      <c r="C55">
+        <v>41.69</v>
+      </c>
+      <c r="D55">
+        <v>40.22</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55">
+        <v>36.9</v>
+      </c>
+      <c r="H55">
+        <v>35.840000000000003</v>
+      </c>
+      <c r="I55">
+        <v>34.729999999999997</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L55">
+        <v>40.46</v>
+      </c>
+      <c r="M55">
+        <v>40.43</v>
+      </c>
+      <c r="N55">
+        <v>40.369999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56">
+        <v>52.82</v>
+      </c>
+      <c r="C56">
+        <v>52.26</v>
+      </c>
+      <c r="D56">
+        <v>51.37</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56">
+        <v>47.07</v>
+      </c>
+      <c r="H56">
+        <v>46.78</v>
+      </c>
+      <c r="I56">
+        <v>46.44</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L56">
+        <v>21.94</v>
+      </c>
+      <c r="M56">
+        <v>21.92</v>
+      </c>
+      <c r="N56">
+        <v>21.87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57">
+        <v>24.76</v>
+      </c>
+      <c r="C57">
+        <v>24.51</v>
+      </c>
+      <c r="D57">
+        <v>24.02</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57">
+        <v>59.82</v>
+      </c>
+      <c r="H57">
+        <v>58.69</v>
+      </c>
+      <c r="I57">
+        <v>57.79</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L57">
+        <v>53.6</v>
+      </c>
+      <c r="M57">
+        <v>53.46</v>
+      </c>
+      <c r="N57">
+        <v>53.38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58">
+        <v>55.42</v>
+      </c>
+      <c r="C58">
+        <v>54.13</v>
+      </c>
+      <c r="D58">
+        <v>53.26</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G58">
+        <f>AVERAGE(G52:G57)</f>
+        <v>45.288333333333334</v>
+      </c>
+      <c r="H58">
+        <f>AVERAGE(H52:H57)</f>
+        <v>44.343333333333334</v>
+      </c>
+      <c r="I58">
+        <f>AVERAGE(I52:I57)</f>
+        <v>43.448333333333331</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L58">
+        <f>AVERAGE(L54:L57)</f>
+        <v>37.482500000000002</v>
+      </c>
+      <c r="M58">
+        <f>AVERAGE(M54:M57)</f>
+        <v>37.412500000000001</v>
+      </c>
+      <c r="N58">
+        <f>AVERAGE(N54:N57)</f>
+        <v>37.347500000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B59">
+        <f>AVERAGE(B52:B58)</f>
+        <v>40.799999999999997</v>
+      </c>
+      <c r="C59">
+        <f>AVERAGE(C52:C58)</f>
+        <v>40.071428571428569</v>
+      </c>
+      <c r="D59">
+        <f>AVERAGE(D52:D58)</f>
+        <v>39.352857142857147</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G59">
+        <f>AVERAGE(G39:G51)</f>
+        <v>49.012307692307687</v>
+      </c>
+      <c r="H59">
+        <f>AVERAGE(H39:H51)</f>
+        <v>48.028461538461542</v>
+      </c>
+      <c r="I59">
+        <f>AVERAGE(I39:I51)</f>
+        <v>47.55</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L59">
+        <f>AVERAGE(L39:L53)</f>
+        <v>39.31066666666667</v>
+      </c>
+      <c r="M59">
+        <f>AVERAGE(M39:M53)</f>
+        <v>39.207333333333331</v>
+      </c>
+      <c r="N59">
+        <f>AVERAGE(N39:N53)</f>
+        <v>39.138000000000012</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60">
+        <f>AVERAGE(B39:B51)</f>
+        <v>41.425384615384615</v>
+      </c>
+      <c r="C60">
+        <f>AVERAGE(C39:C51)</f>
+        <v>40.5523076923077</v>
+      </c>
+      <c r="D60">
+        <f>AVERAGE(D39:D51)</f>
+        <v>40.123846153846145</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60">
+        <f>AVERAGE(G39:G57)</f>
+        <v>47.836315789473687</v>
+      </c>
+      <c r="H60">
+        <f>AVERAGE(H39:H57)</f>
+        <v>46.864736842105266</v>
+      </c>
+      <c r="I60">
+        <f>AVERAGE(I39:I57)</f>
+        <v>46.25473684210526</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L60">
+        <f>AVERAGE(L39:L57)</f>
+        <v>38.925789473684219</v>
+      </c>
+      <c r="M60">
+        <f>AVERAGE(M39:M57)</f>
+        <v>38.829473684210527</v>
+      </c>
+      <c r="N60">
+        <f>AVERAGE(N39:N57)</f>
+        <v>38.761052631578956</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B61">
+        <f>AVERAGE(B39:B58)</f>
+        <v>41.206499999999998</v>
+      </c>
+      <c r="C61">
+        <f>AVERAGE(C39:C58)</f>
+        <v>40.384</v>
+      </c>
+      <c r="D61">
+        <f>AVERAGE(D39:D58)</f>
+        <v>39.853999999999992</v>
+      </c>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F64" s="4"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B67" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="L67" s="13"/>
+      <c r="M67" s="13"/>
+      <c r="N67" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="O67" s="13"/>
+      <c r="P67" s="13"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O68" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="P68" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B69">
+        <v>31.86</v>
+      </c>
+      <c r="C69">
+        <v>31.91</v>
+      </c>
+      <c r="D69">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="E69">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="F69">
+        <v>35.229999999999997</v>
+      </c>
+      <c r="G69">
+        <v>35.119999999999997</v>
+      </c>
+      <c r="H69">
+        <v>29.78</v>
+      </c>
+      <c r="I69">
+        <v>28.76</v>
+      </c>
+      <c r="J69">
+        <v>29.8</v>
+      </c>
+      <c r="K69">
+        <v>34.14</v>
+      </c>
+      <c r="L69">
+        <v>32.97</v>
+      </c>
+      <c r="M69">
+        <v>34.24</v>
+      </c>
+      <c r="N69">
+        <v>51.52</v>
+      </c>
+      <c r="O69">
+        <v>49.75</v>
+      </c>
+      <c r="P69">
+        <v>51.97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B71" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="M71" s="13"/>
+      <c r="N71" s="13"/>
+      <c r="O71" s="13"/>
+      <c r="P71" s="13"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="L72" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M72" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N72" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="O72" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P72" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73">
+        <v>29.78</v>
+      </c>
+      <c r="C73">
+        <v>31.86</v>
+      </c>
+      <c r="D73">
+        <v>34.14</v>
+      </c>
+      <c r="E73">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="F73">
+        <v>51.52</v>
+      </c>
+      <c r="G73">
+        <v>28.76</v>
+      </c>
+      <c r="H73">
+        <v>31.91</v>
+      </c>
+      <c r="I73">
+        <v>32.97</v>
+      </c>
+      <c r="J73">
+        <v>35.229999999999997</v>
+      </c>
+      <c r="K73">
+        <v>49.75</v>
+      </c>
+      <c r="L73">
+        <v>29.8</v>
+      </c>
+      <c r="M73">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="N73">
+        <v>34.24</v>
+      </c>
+      <c r="O73">
+        <v>35.119999999999997</v>
+      </c>
+      <c r="P73">
+        <v>51.97</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13"/>
+      <c r="O76" s="13"/>
+      <c r="P76" s="13"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+    </row>
+  </sheetData>
+  <sortState ref="B73:F73">
+    <sortCondition ref="B72"/>
+  </sortState>
+  <mergeCells count="20">
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="G76:K76"/>
+    <mergeCell ref="L76:P76"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="G71:K71"/>
+    <mergeCell ref="L71:P71"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="H67:J67"/>
+    <mergeCell ref="K67:M67"/>
+    <mergeCell ref="N67:P67"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A2:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="U34" sqref="U34"/>
     </sheetView>
   </sheetViews>
@@ -55339,27 +58422,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="I2" s="14" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="O2" s="14" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="O2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
       <c r="S2" s="4"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -57547,22 +60630,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -57581,24 +60664,24 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="15" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="18"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -61223,14 +64306,14 @@
       <c r="N2" s="4">
         <v>512</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -63616,22 +66699,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -64993,22 +68076,22 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
@@ -67132,14 +70215,14 @@
       <c r="N2" s="4">
         <v>500</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -69438,22 +72521,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -70662,14 +73745,14 @@
       <c r="A34" s="4"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>

</xml_diff>

<commit_message>
Removed the pdf file from the repo since it causes issues when collaborating. Added some of Mitesh's comments
</commit_message>
<xml_diff>
--- a/paper/raw_data/results_HBM2_DDR41600_and_offline.xlsx
+++ b/paper/raw_data/results_HBM2_DDR41600_and_offline.xlsx
@@ -314,7 +314,7 @@
     <t>HMA 0.01</t>
   </si>
   <si>
-    <t>HMA OCL</t>
+    <t>HMA OPT</t>
   </si>
 </sst>
 </file>
@@ -18043,7 +18043,7 @@
                 <c:ptCount val="15"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>HMA OCL</c:v>
+                    <c:v>HMA OPT</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>MP</c:v>
@@ -18058,7 +18058,7 @@
                     <c:v>HMA 0.05</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>HMA OCL</c:v>
+                    <c:v>HMA OPT</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>MP</c:v>
@@ -18073,7 +18073,7 @@
                     <c:v>HMA 0.05</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>HMA OCL</c:v>
+                    <c:v>HMA OPT</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>MP</c:v>
@@ -18139,19 +18139,19 @@
                   <c:v>49.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29.8</c:v>
+                  <c:v>27.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>30.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.24</c:v>
+                  <c:v>32.24</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35.119999999999997</c:v>
+                  <c:v>33.119999999999997</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>51.97</c:v>
+                  <c:v>49.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18201,10 +18201,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -18251,10 +18248,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -18284,10 +18278,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -18316,10 +18307,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -18365,7 +18353,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -18373,7 +18365,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -42060,16 +42052,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -56298,7 +56290,7 @@
   <dimension ref="A1:V77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="M72" sqref="M72"/>
+      <selection activeCell="T64" sqref="T64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58330,19 +58322,31 @@
         <v>49.75</v>
       </c>
       <c r="L73">
-        <v>29.8</v>
+        <v>27.8</v>
       </c>
       <c r="M73">
-        <v>32.299999999999997</v>
+        <v>30.299999999999997</v>
       </c>
       <c r="N73">
-        <v>34.24</v>
+        <v>32.24</v>
       </c>
       <c r="O73">
-        <v>35.119999999999997</v>
+        <v>33.119999999999997</v>
       </c>
       <c r="P73">
-        <v>51.97</v>
+        <v>49.7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M74">
+        <f>M73/N73</f>
+        <v>0.93982630272952838</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M75">
+        <f>M73/O73</f>
+        <v>0.91485507246376807</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -58356,11 +58360,14 @@
       <c r="I76" s="13"/>
       <c r="J76" s="13"/>
       <c r="K76" s="13"/>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-      <c r="N76" s="13"/>
-      <c r="O76" s="13"/>
-      <c r="P76" s="13"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9">
+        <f>M73/P73</f>
+        <v>0.60965794768611659</v>
+      </c>
+      <c r="N76" s="9"/>
+      <c r="O76" s="9"/>
+      <c r="P76" s="9"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
@@ -58368,15 +58375,18 @@
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
+      <c r="M77">
+        <f>M73/L73</f>
+        <v>1.0899280575539567</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B73:F73">
     <sortCondition ref="B72"/>
   </sortState>
-  <mergeCells count="20">
+  <mergeCells count="19">
     <mergeCell ref="B76:F76"/>
     <mergeCell ref="G76:K76"/>
-    <mergeCell ref="L76:P76"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>

</xml_diff>